<commit_message>
arr/act completed, added bernuolli & new struct for arr/ST
</commit_message>
<xml_diff>
--- a/relations.xlsx
+++ b/relations.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fifteen\.julia\dev\ArrhythmRelations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="384" yWindow="456" windowWidth="28044" windowHeight="17040"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Load" sheetId="1" r:id="rId1"/>
+    <sheet name="Sense" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,8 +24,73 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="20">
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Fisher QRS</t>
+  </si>
+  <si>
+    <t>Fisher 10s</t>
+  </si>
+  <si>
+    <t>Fisher 60s</t>
+  </si>
+  <si>
+    <t>Chi2 QRS</t>
+  </si>
+  <si>
+    <t>Chi2 10s</t>
+  </si>
+  <si>
+    <t>Chi2 60s</t>
+  </si>
+  <si>
+    <t>Binom QRS</t>
+  </si>
+  <si>
+    <t>Binom 10s</t>
+  </si>
+  <si>
+    <t>Binom 60s</t>
+  </si>
+  <si>
+    <t>Percent QRS</t>
+  </si>
+  <si>
+    <t>Percent 10s</t>
+  </si>
+  <si>
+    <t>Percent 60s</t>
+  </si>
+  <si>
+    <t>ChildArithm.avt</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Ishem_Arithm.avt</t>
+  </si>
+  <si>
+    <t>ReoBreath.avt</t>
+  </si>
+  <si>
+    <t>Seminar_AD_FP.avt</t>
+  </si>
+  <si>
+    <t>VMT_Arrh_101159.avt</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -35,12 +100,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -55,11 +132,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -370,13 +449,359 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
task 3 (arr/ST) completed with tests
</commit_message>
<xml_diff>
--- a/relations.xlsx
+++ b/relations.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fifteen\.julia\dev\ArrhythmRelations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="456" windowWidth="28044" windowHeight="17040"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Load" sheetId="1" r:id="rId1"/>
-    <sheet name="Sense" sheetId="2" r:id="rId2"/>
+    <sheet name="Sense" r:id="rId4" sheetId="2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>Filename</t>
   </si>
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -100,24 +101,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -132,13 +121,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -449,16 +436,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,208 +484,208 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" s="2" t="s">
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -710,16 +695,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -760,44 +743,44 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="2" t="s">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>